<commit_message>
Remove duplicate entries for Analog pins
Remove duplicate entries for Analog pins
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -11,15 +11,15 @@
     <sheet name="Pinout for 1.0A " sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pinout for 1.0 and 2.0'!$A$1:$H$144</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pinout for 1.0A '!$A$1:$H$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pinout for 1.0A '!$A$1:$H$137</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -1614,10 +1614,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K144"/>
+  <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129:G129"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,52 +2996,46 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" s="12">
-        <v>79</v>
-      </c>
-      <c r="D57" s="12">
-        <v>55</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="H57" s="18">
-        <v>11</v>
+      <c r="A57" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C57" s="2">
+        <v>78</v>
+      </c>
+      <c r="D57" s="24">
+        <v>54</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C58" s="12">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" s="12">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>158</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H58" s="18">
         <v>11</v>
@@ -3049,516 +3043,574 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C59" s="12">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D59" s="12">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>158</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H59" s="18">
         <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C60" s="12">
+        <v>81</v>
+      </c>
+      <c r="D60" s="12">
+        <v>57</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H60" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C61" s="2">
         <v>82</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D61" s="2">
         <v>58</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G61" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="H60" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2">
+      <c r="H61" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C62" s="2">
+        <v>83</v>
+      </c>
+      <c r="D62" s="24">
         <v>59</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2">
-        <v>60</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="18">
+      <c r="G62" s="2"/>
+      <c r="H62" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2">
-        <v>61</v>
+      <c r="A63" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C63" s="2">
+        <v>84</v>
+      </c>
+      <c r="D63" s="24">
+        <v>60</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="18">
+      <c r="G63" s="2"/>
+      <c r="H63" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2">
-        <v>62</v>
+      <c r="A64" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C64" s="2">
+        <v>85</v>
+      </c>
+      <c r="D64" s="24">
+        <v>61</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2">
+      <c r="G64" s="2"/>
+      <c r="H64" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C65" s="2">
+        <v>88</v>
+      </c>
+      <c r="D65" s="24">
+        <v>62</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C66" s="3">
+        <v>89</v>
+      </c>
+      <c r="D66" s="25">
         <v>63</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2">
+      <c r="E66" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H66" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C67" s="2">
+        <v>90</v>
+      </c>
+      <c r="D67" s="24">
         <v>64</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="E67" s="2"/>
+      <c r="F67" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B68" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C68" s="11">
         <v>91</v>
       </c>
-      <c r="D67" s="11">
+      <c r="D68" s="11">
         <v>65</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E68" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F68" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G68" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="H67" s="18">
+      <c r="H68" s="18">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C69" s="2">
         <v>76</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D69" s="2">
         <v>66</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="G69" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="H68" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="H69" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C70" s="2">
         <v>77</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D70" s="2">
         <v>67</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G69" s="19"/>
-      <c r="H69" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+      <c r="G70" s="19"/>
+      <c r="H70" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B71" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C71" s="10">
         <v>24</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D71" s="10">
         <v>68</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="E71" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F71" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G70" s="10" t="s">
+      <c r="G71" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="H70" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" s="10">
-        <v>23</v>
-      </c>
-      <c r="D71" s="10">
-        <v>69</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>218</v>
       </c>
       <c r="H71" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C72" s="10">
+        <v>23</v>
+      </c>
+      <c r="D72" s="10">
+        <v>69</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="H72" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B73" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>9</v>
       </c>
-      <c r="D72" s="5">
+      <c r="D73" s="5">
         <v>70</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F73" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G73" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="H72" s="18">
+      <c r="H73" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C74" s="2">
         <v>70</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D74" s="2">
         <v>71</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C74" s="8">
+      <c r="C75" s="8">
         <v>103</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D75" s="8">
         <v>72</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E75" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F75" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G74" s="8" t="s">
+      <c r="G75" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="H74" s="18">
+      <c r="H75" s="18">
         <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C75" s="12">
-        <v>107</v>
-      </c>
-      <c r="D75" s="12">
-        <v>73</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="H75" s="18">
-        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C76" s="12">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D76" s="12">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>230</v>
+        <v>158</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H76" s="18">
         <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C77" s="8">
-        <v>109</v>
-      </c>
-      <c r="D77" s="8">
-        <v>75</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>235</v>
+      <c r="A77" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" s="12">
+        <v>108</v>
+      </c>
+      <c r="D77" s="12">
+        <v>74</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>232</v>
       </c>
       <c r="H77" s="18">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C78" s="8">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D78" s="8">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>46</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H78" s="18">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C79" s="8">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D79" s="8">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>46</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H79" s="18">
         <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C80" s="8">
+        <v>111</v>
+      </c>
+      <c r="D80" s="8">
+        <v>77</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H80" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B81" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C80" s="14">
+      <c r="C81" s="14">
         <v>142</v>
       </c>
-      <c r="D80" s="14">
+      <c r="D81" s="14">
         <v>78</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E81" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F80" s="14" t="s">
+      <c r="F81" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="G80" s="14" t="s">
+      <c r="G81" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="H80" s="18">
+      <c r="H81" s="18">
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2">
-        <v>79</v>
-      </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -3567,12 +3619,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -3581,12 +3633,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -3595,12 +3647,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
@@ -3609,12 +3661,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -3623,92 +3675,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2">
+        <v>84</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B88" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C87" s="14">
+      <c r="C88" s="14">
         <v>129</v>
       </c>
-      <c r="D87" s="14">
+      <c r="D88" s="14">
         <v>85</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E88" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="F87" s="14" t="s">
+      <c r="F88" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G87" s="14" t="s">
+      <c r="G88" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="H87" s="18">
+      <c r="H88" s="18">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2">
         <v>86</v>
       </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C90" s="2">
         <v>112</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D90" s="2">
         <v>87</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G89" s="19" t="s">
+      <c r="G90" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="H89" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2">
-        <v>88</v>
-      </c>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="19"/>
       <c r="H90" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -3717,12 +3769,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -3730,13 +3782,16 @@
       <c r="H92" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -3744,13 +3799,16 @@
       <c r="H93" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -3758,13 +3816,16 @@
       <c r="H94" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -3773,12 +3834,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -3787,12 +3848,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -3801,12 +3862,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -3814,16 +3875,13 @@
       <c r="H98" s="18">
         <v>0</v>
       </c>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-      <c r="K98" s="15"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -3831,16 +3889,13 @@
       <c r="H99" s="18">
         <v>0</v>
       </c>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
-      <c r="K99" s="15"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -3848,16 +3903,13 @@
       <c r="H100" s="18">
         <v>0</v>
       </c>
-      <c r="I100" s="15"/>
-      <c r="J100" s="15"/>
-      <c r="K100" s="15"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -3866,52 +3918,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2">
+        <v>99</v>
+      </c>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C103" s="2">
         <v>25</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D103" s="2">
         <v>100</v>
       </c>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2" t="s">
+      <c r="E103" s="2"/>
+      <c r="F103" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G102" s="19" t="s">
+      <c r="G103" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="H102" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="H103" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2">
         <v>138</v>
       </c>
-      <c r="D103" s="2">
-        <v>101</v>
-      </c>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="19"/>
-      <c r="H103" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
       <c r="D104" s="2">
         <v>101</v>
       </c>
@@ -3922,12 +3974,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -3936,60 +3988,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19">
-        <v>103</v>
-      </c>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2">
+        <v>102</v>
+      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="19"/>
       <c r="H106" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="19"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19">
+        <v>103</v>
+      </c>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2">
         <v>93</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D108" s="2">
         <v>104</v>
       </c>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2" t="s">
+      <c r="E108" s="2"/>
+      <c r="F108" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G107" s="2"/>
-      <c r="H107" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="19"/>
-      <c r="B108" s="19"/>
-      <c r="C108" s="19"/>
-      <c r="D108" s="19">
-        <v>105</v>
-      </c>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="19"/>
+      <c r="G108" s="2"/>
       <c r="H108" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="19"/>
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
       <c r="D109" s="19">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E109" s="19"/>
       <c r="F109" s="19"/>
@@ -3998,12 +4050,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="19"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
       <c r="D110" s="19">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E110" s="19"/>
       <c r="F110" s="19"/>
@@ -4012,40 +4064,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="19"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19">
+        <v>107</v>
+      </c>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2">
+      <c r="B112" s="2"/>
+      <c r="C112" s="2">
         <v>131</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D112" s="2">
         <v>108</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E112" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G111" s="2"/>
-      <c r="H111" s="18">
+      <c r="G112" s="2"/>
+      <c r="H112" s="18">
         <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="19"/>
-      <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19">
-        <v>109</v>
-      </c>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="19"/>
-      <c r="H112" s="18">
-        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4053,7 +4105,7 @@
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
       <c r="D113" s="19">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
@@ -4067,7 +4119,7 @@
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
       <c r="D114" s="19">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E114" s="19"/>
       <c r="F114" s="19"/>
@@ -4081,7 +4133,7 @@
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
       <c r="D115" s="19">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E115" s="19"/>
       <c r="F115" s="19"/>
@@ -4095,7 +4147,7 @@
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
       <c r="D116" s="19">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E116" s="19"/>
       <c r="F116" s="19"/>
@@ -4109,7 +4161,7 @@
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
       <c r="D117" s="19">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E117" s="19"/>
       <c r="F117" s="19"/>
@@ -4119,130 +4171,118 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="B118" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="C118" s="21">
-        <v>113</v>
-      </c>
-      <c r="D118" s="21">
-        <v>115</v>
-      </c>
-      <c r="E118" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="F118" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="G118" s="21" t="s">
-        <v>262</v>
-      </c>
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19">
+        <v>114</v>
+      </c>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
       <c r="H118" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="21" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C119" s="21">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D119" s="21">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F119" s="21" t="s">
         <v>261</v>
       </c>
       <c r="G119" s="21" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H119" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="C120" s="21">
+        <v>114</v>
+      </c>
+      <c r="D120" s="21">
+        <v>116</v>
+      </c>
+      <c r="E120" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="F120" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G120" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="H120" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C120" s="4">
+      <c r="C121" s="4">
         <v>115</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <v>117</v>
       </c>
-      <c r="E120" s="4" t="s">
+      <c r="E121" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="F121" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="G120" s="4" t="s">
+      <c r="G121" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H120" s="18">
+      <c r="H121" s="18">
         <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B121" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="C121" s="22">
-        <v>118</v>
-      </c>
-      <c r="D121" s="22">
-        <v>118</v>
-      </c>
-      <c r="E121" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="F121" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G121" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="H121" s="18">
-        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="22" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C122" s="22">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D122" s="22">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E122" s="22" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F122" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G122" s="22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H122" s="18">
         <v>13</v>
@@ -4250,77 +4290,77 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C123" s="22">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D123" s="22">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E123" s="22" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F123" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G123" s="22" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H123" s="18">
         <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="B124" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="C124" s="11">
-        <v>121</v>
-      </c>
-      <c r="D124" s="11">
-        <v>121</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="F124" s="11" t="s">
+      <c r="A124" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B124" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C124" s="22">
+        <v>120</v>
+      </c>
+      <c r="D124" s="22">
+        <v>120</v>
+      </c>
+      <c r="E124" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F124" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G124" s="11" t="s">
-        <v>286</v>
+      <c r="G124" s="22" t="s">
+        <v>282</v>
       </c>
       <c r="H124" s="18">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C125" s="11">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D125" s="11">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F125" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H125" s="18">
         <v>14</v>
@@ -4328,191 +4368,193 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C126" s="11">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D126" s="11">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F126" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H126" s="18">
         <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="22" t="s">
+      <c r="A127" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C127" s="11">
+        <v>123</v>
+      </c>
+      <c r="D127" s="11">
+        <v>123</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="H127" s="18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="B127" s="22" t="s">
+      <c r="B128" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C127" s="22">
+      <c r="C128" s="22">
         <v>2</v>
       </c>
-      <c r="D127" s="22">
+      <c r="D128" s="22">
         <v>124</v>
       </c>
-      <c r="E127" s="22" t="s">
+      <c r="E128" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="F127" s="22" t="s">
+      <c r="F128" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G127" s="22" t="s">
+      <c r="G128" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="H127" s="17">
+      <c r="H128" s="17">
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="7" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B129" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C128" s="7">
+      <c r="C129" s="7">
         <v>143</v>
       </c>
-      <c r="D128" s="7">
+      <c r="D129" s="7">
         <v>125</v>
       </c>
-      <c r="E128" s="7" t="s">
+      <c r="E129" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="F129" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="G128" s="7" t="s">
+      <c r="G129" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="H128" s="17">
+      <c r="H129" s="17">
         <v>10</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3">
-        <v>141</v>
-      </c>
-      <c r="D129" s="3">
-        <v>128</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
-      <c r="H129" s="17">
-        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>306</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="B130" s="3"/>
       <c r="C130" s="3">
+        <v>141</v>
+      </c>
+      <c r="D130" s="3">
         <v>128</v>
       </c>
-      <c r="D130" s="3">
-        <v>129</v>
-      </c>
       <c r="E130" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>308</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
       <c r="H130" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C131" s="3">
+        <v>128</v>
+      </c>
+      <c r="D131" s="3">
+        <v>129</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="H131" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="C131" s="4">
+      <c r="C132" s="4">
         <v>92</v>
       </c>
-      <c r="D131" s="23" t="s">
+      <c r="D132" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E132" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="F131" s="4" t="s">
+      <c r="F132" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G131" s="4" t="s">
+      <c r="G132" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="H131" s="17">
+      <c r="H132" s="17">
         <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C132" s="2">
-        <v>78</v>
-      </c>
-      <c r="D132" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="C133" s="2">
-        <v>90</v>
-      </c>
-      <c r="D133" s="24" t="s">
-        <v>317</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D133" s="2"/>
       <c r="E133" s="2"/>
-      <c r="F133" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="F133" s="2"/>
       <c r="G133" s="2"/>
       <c r="H133" s="17">
         <v>0</v>
@@ -4520,17 +4562,15 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C134" s="2">
-        <v>83</v>
-      </c>
-      <c r="D134" s="24" t="s">
-        <v>319</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -4540,17 +4580,15 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="C135" s="2">
-        <v>84</v>
-      </c>
-      <c r="D135" s="24" t="s">
-        <v>321</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -4560,17 +4598,15 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="C136" s="2">
-        <v>85</v>
-      </c>
-      <c r="D136" s="24" t="s">
-        <v>323</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D136" s="2"/>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -4580,160 +4616,40 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>325</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="B137" s="2"/>
       <c r="C137" s="2">
-        <v>88</v>
-      </c>
-      <c r="D137" s="24" t="s">
-        <v>325</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="F137" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="F137" s="2"/>
       <c r="G137" s="2"/>
       <c r="H137" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C138" s="3">
-        <v>89</v>
-      </c>
-      <c r="D138" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>329</v>
-      </c>
+      <c r="A138" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C138" s="2">
+        <v>130</v>
+      </c>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
       <c r="H138" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C139" s="2">
-        <v>28</v>
-      </c>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
-      <c r="H139" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C140" s="2">
-        <v>29</v>
-      </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C141" s="2">
-        <v>30</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C142" s="2">
-        <v>31</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2">
-        <v>117</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C144" s="2">
-        <v>130</v>
-      </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
-      <c r="G144" s="2"/>
-      <c r="H144" s="17">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H144">
+  <autoFilter ref="A1:H138">
     <sortState ref="A2:H144">
       <sortCondition ref="D1:D144"/>
     </sortState>
@@ -4748,17 +4664,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K144"/>
+  <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="13"/>
     <col min="4" max="4" width="20.28515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="17" style="13" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="13" customWidth="1"/>
     <col min="7" max="7" width="70.28515625" style="13" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" style="16" customWidth="1"/>
@@ -6114,16 +6030,22 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2">
+      <c r="A56" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C56" s="2">
+        <v>78</v>
+      </c>
+      <c r="D56" s="24">
         <v>54</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="18">
+      <c r="G56" s="2"/>
+      <c r="H56" s="17">
         <v>0</v>
       </c>
     </row>
@@ -6232,86 +6154,132 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2">
+      <c r="A61" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C61" s="2">
+        <v>83</v>
+      </c>
+      <c r="D61" s="24">
         <v>59</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="18">
+      <c r="G61" s="2"/>
+      <c r="H61" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2">
+      <c r="A62" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C62" s="2">
+        <v>84</v>
+      </c>
+      <c r="D62" s="24">
         <v>60</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="18">
+      <c r="G62" s="2"/>
+      <c r="H62" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2">
+      <c r="A63" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" s="2">
+        <v>85</v>
+      </c>
+      <c r="D63" s="24">
         <v>61</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="18">
+      <c r="G63" s="2"/>
+      <c r="H63" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2">
+      <c r="A64" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C64" s="2">
+        <v>88</v>
+      </c>
+      <c r="D64" s="24">
         <v>62</v>
       </c>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="18">
+      <c r="F64" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2">
+      <c r="A65" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C65" s="3">
+        <v>89</v>
+      </c>
+      <c r="D65" s="25">
         <v>63</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="18">
-        <v>0</v>
+      <c r="E65" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H65" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2">
+      <c r="A66" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C66" s="2">
+        <v>90</v>
+      </c>
+      <c r="D66" s="24">
         <v>64</v>
       </c>
       <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="18">
+      <c r="F66" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="17">
         <v>0</v>
       </c>
     </row>
@@ -6593,7 +6561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>236</v>
       </c>
@@ -6671,7 +6639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -6685,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -6699,7 +6667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -6713,7 +6681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -6727,7 +6695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -6741,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -6755,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="26" t="s">
         <v>246</v>
       </c>
@@ -6775,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -6789,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>249</v>
       </c>
@@ -6815,7 +6783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -6829,7 +6797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -6842,8 +6810,11 @@
       <c r="H91" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -6856,8 +6827,11 @@
       <c r="H92" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -6870,8 +6844,11 @@
       <c r="H93" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -6885,7 +6862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -6899,7 +6876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -6913,7 +6890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -6927,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -6940,11 +6917,8 @@
       <c r="H98" s="18">
         <v>0</v>
       </c>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-      <c r="K98" s="15"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -6957,11 +6931,8 @@
       <c r="H99" s="18">
         <v>0</v>
       </c>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
-      <c r="K99" s="15"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -6974,11 +6945,8 @@
       <c r="H100" s="18">
         <v>0</v>
       </c>
-      <c r="I100" s="15"/>
-      <c r="J100" s="15"/>
-      <c r="K100" s="15"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -6992,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>252</v>
       </c>
@@ -7016,7 +6984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>255</v>
       </c>
@@ -7034,7 +7002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7048,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7062,7 +7030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="19"/>
       <c r="B106" s="19"/>
       <c r="C106" s="19"/>
@@ -7076,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>256</v>
       </c>
@@ -7096,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="19"/>
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
@@ -7110,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="19"/>
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
@@ -7124,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="19"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
@@ -7138,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>257</v>
       </c>
@@ -7160,7 +7128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="19"/>
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
@@ -7602,17 +7570,15 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>315</v>
+        <v>339</v>
       </c>
       <c r="C132" s="2">
-        <v>78</v>
-      </c>
-      <c r="D132" s="24" t="s">
-        <v>315</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -7622,21 +7588,15 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>317</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="B133" s="2"/>
       <c r="C133" s="2">
-        <v>90</v>
-      </c>
-      <c r="D133" s="24" t="s">
-        <v>317</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D133" s="2"/>
       <c r="E133" s="2"/>
-      <c r="F133" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="F133" s="2"/>
       <c r="G133" s="2"/>
       <c r="H133" s="17">
         <v>0</v>
@@ -7644,17 +7604,15 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="C134" s="2">
-        <v>83</v>
-      </c>
-      <c r="D134" s="24" t="s">
-        <v>319</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -7664,17 +7622,15 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="C135" s="2">
-        <v>84</v>
-      </c>
-      <c r="D135" s="24" t="s">
-        <v>321</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -7684,17 +7640,15 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C136" s="2">
-        <v>85</v>
-      </c>
-      <c r="D136" s="24" t="s">
-        <v>323</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D136" s="2"/>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -7704,162 +7658,26 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="C137" s="2">
-        <v>88</v>
-      </c>
-      <c r="D137" s="24" t="s">
-        <v>325</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="F137" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="F137" s="2"/>
       <c r="G137" s="2"/>
       <c r="H137" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C138" s="3">
-        <v>89</v>
-      </c>
-      <c r="D138" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="H138" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C139" s="2">
-        <v>130</v>
-      </c>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
-      <c r="H139" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2">
-        <v>117</v>
-      </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C141" s="2">
-        <v>31</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C142" s="2">
-        <v>30</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C143" s="2">
-        <v>29</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C144" s="2">
-        <v>28</v>
-      </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
-      <c r="G144" s="2"/>
-      <c r="H144" s="17">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H144">
-    <sortState ref="A2:H144">
-      <sortCondition ref="D1:D144"/>
+  <autoFilter ref="A1:H137">
+    <sortState ref="A2:H139">
+      <sortCondition ref="D1:D139"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update for 2.0A still one pin missing: E1 enable
Update for 2.0A still one pin missing: E1 enable pin, can be 124, 85 or
any free pin
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout for 1.0 and 2.0" sheetId="2" r:id="rId1"/>
-    <sheet name="Pinout for 1.0A " sheetId="3" r:id="rId2"/>
+    <sheet name="Pinout for 1.0A and 2,0A " sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pinout for 1.0A '!$A$1:$H$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pinout for 1.0A and 2,0A '!$A$1:$H$137</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
@@ -1322,6 +1322,124 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12344400" y="2133600"/>
+          <a:ext cx="2800350" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Miss</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Pin for 2.0A</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Motor E2 enable, 0 = enable</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="1" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Can be 124, 85 or any free one</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1616,8 +1734,8 @@
   </sheetPr>
   <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4666,8 +4784,8 @@
   </sheetPr>
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7682,5 +7800,6 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for AiO door sensor / badge light
Thanks @kryts for helping providing pins and behavior
Badge light follow global light behavior but in addition it can be
switched off independently in settings/EEPROM

need some code refactoring as a lot of redondant code - but later...
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout for 1.0 and 2.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,18 +19,21 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Pinout for 1.0 and 2.0'!$A$1:$H$138</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Pinout for 1.0A and 2,0A '!$A$1:$H$137</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Pinout for 1.0A and 2,0A '!$A$1:$H$137</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Pinout for 1.0A and 2,0A '!$A$1:$H$137</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Pinout for 1.0A and 2,0A '!$A$1:$H$137</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">AiO!$A$1:$H$137</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">AiO!$A$1:$H$137</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">AiO!$A$1:$H$137</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="347">
   <si>
     <t>NAME</t>
   </si>
@@ -1065,6 +1068,12 @@
   </si>
   <si>
     <t>ERASE S</t>
+  </si>
+  <si>
+    <t>Badge LED,  1 = On</t>
+  </si>
+  <si>
+    <t>PC24,135,6,Badge LED,  1 = On</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1083,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1102,6 +1111,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1250,7 +1265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1355,6 +1370,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1440,15 +1459,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
+      <xdr:colOff>325800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>504720</xdr:colOff>
+      <xdr:colOff>531360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1457,8 +1476,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13099680" y="2268360"/>
-          <a:ext cx="3431520" cy="1733400"/>
+          <a:off x="13126680" y="2259360"/>
+          <a:ext cx="3431160" cy="1733040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7649,8 +7668,8 @@
   </sheetPr>
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D130" activeCellId="0" sqref="D130"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7853,14 +7872,12 @@
       <c r="D8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="E8" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>36</v>
+        <v>346</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>4</v>
@@ -9257,7 +9274,9 @@
       <c r="D66" s="18" t="n">
         <v>64</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F66" s="2" t="s">
         <v>213</v>
       </c>
@@ -10499,7 +10518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="7" t="s">
         <v>326</v>
       </c>

</xml_diff>

<commit_message>
Add pins for Lasers / calibration leds/ turntable
Thanks @zeus10
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc.VAIO\Documents\GitHub\Repetier-Firmware-0.92\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout for 1.0 and 2.0" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="354">
   <si>
     <t>NAME</t>
   </si>
@@ -1070,13 +1075,41 @@
   </si>
   <si>
     <t>PC24,135,6,Badge LED,  1 = On</t>
+  </si>
+  <si>
+    <t>Turn Table direction, 0=-, 1=+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>White Led Laser 1, 1=0n</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laser 2, 1 = 0N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn Table step</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn Table enable, 0 = enable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laser 1, 1 = ON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>White Led Laser 2, 1=ON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1096,8 +1129,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1194,6 +1233,18 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFC4BD97"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1222,7 +1273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1266,9 +1317,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1344,12 +1398,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1391,7 +1448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1426,7 +1483,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1644,20 +1701,18 @@
       <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125"/>
-    <col min="2" max="2" width="11.7109375"/>
-    <col min="3" max="3" width="8.7109375"/>
+    <col min="1" max="1" width="15.453125"/>
+    <col min="2" max="2" width="11.7265625"/>
     <col min="4" max="4" width="18"/>
-    <col min="5" max="5" width="46.5703125"/>
+    <col min="5" max="5" width="46.54296875"/>
     <col min="6" max="6" width="30"/>
-    <col min="7" max="7" width="71.7109375"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
-    <col min="9" max="1025" width="8.7109375"/>
+    <col min="7" max="7" width="71.7265625"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1757,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1781,7 +1836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1807,7 +1862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -1833,7 +1888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -1885,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -1911,7 +1966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1933,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -1959,7 +2014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -1985,7 +2040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -2011,7 +2066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
@@ -2035,7 +2090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -2061,7 +2116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -2087,7 +2142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -2113,7 +2168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -2139,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -2161,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -2183,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -2209,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -2231,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -2255,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -2281,7 +2336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -2307,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -2333,7 +2388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -2355,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -2377,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -2399,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -2425,7 +2480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -2451,7 +2506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -2477,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -2499,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -2523,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -2549,7 +2604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -2575,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -2601,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -2627,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -2653,7 +2708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -2679,7 +2734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -2705,7 +2760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -2757,7 +2812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -2783,7 +2838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -2809,7 +2864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -2835,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -2857,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -2879,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -2901,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -2923,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -2945,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -2967,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2981,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -3007,7 +3062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3021,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>190</v>
       </c>
@@ -3041,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>192</v>
       </c>
@@ -3067,7 +3122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>195</v>
       </c>
@@ -3093,7 +3148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>198</v>
       </c>
@@ -3119,7 +3174,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>201</v>
       </c>
@@ -3145,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -3165,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>207</v>
       </c>
@@ -3185,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>209</v>
       </c>
@@ -3205,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>211</v>
       </c>
@@ -3227,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>214</v>
       </c>
@@ -3253,7 +3308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>218</v>
       </c>
@@ -3275,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
         <v>220</v>
       </c>
@@ -3301,7 +3356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>224</v>
       </c>
@@ -3327,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>228</v>
       </c>
@@ -3351,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>230</v>
       </c>
@@ -3377,7 +3432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="15" t="s">
         <v>234</v>
       </c>
@@ -3403,7 +3458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>238</v>
       </c>
@@ -3429,7 +3484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>241</v>
       </c>
@@ -3449,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
         <v>243</v>
       </c>
@@ -3475,7 +3530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>246</v>
       </c>
@@ -3501,7 +3556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>249</v>
       </c>
@@ -3527,7 +3582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>253</v>
       </c>
@@ -3553,7 +3608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>256</v>
       </c>
@@ -3579,7 +3634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>259</v>
       </c>
@@ -3605,7 +3660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="22" t="s">
         <v>262</v>
       </c>
@@ -3631,7 +3686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3645,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3659,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3673,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3687,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3701,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3715,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="22" t="s">
         <v>266</v>
       </c>
@@ -3741,7 +3796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3755,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>269</v>
       </c>
@@ -3781,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3795,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3812,7 +3867,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3829,7 +3884,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3846,7 +3901,7 @@
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3860,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3874,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3888,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3902,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3916,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3930,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3944,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3958,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>272</v>
       </c>
@@ -3982,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>275</v>
       </c>
@@ -4000,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4014,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4028,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -4042,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>276</v>
       </c>
@@ -4062,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -4076,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -4090,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -4104,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>277</v>
       </c>
@@ -4126,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -4140,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -4154,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -4168,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -4182,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -4196,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -4210,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>279</v>
       </c>
@@ -4236,7 +4291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="23" t="s">
         <v>284</v>
       </c>
@@ -4262,7 +4317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="8" t="s">
         <v>288</v>
       </c>
@@ -4288,7 +4343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>292</v>
       </c>
@@ -4314,7 +4369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>296</v>
       </c>
@@ -4340,7 +4395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="24" t="s">
         <v>300</v>
       </c>
@@ -4366,7 +4421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>304</v>
       </c>
@@ -4392,7 +4447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>308</v>
       </c>
@@ -4418,7 +4473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="16" t="s">
         <v>312</v>
       </c>
@@ -4444,7 +4499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="24" t="s">
         <v>316</v>
       </c>
@@ -4470,7 +4525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
         <v>320</v>
       </c>
@@ -4496,7 +4551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>324</v>
       </c>
@@ -4516,7 +4571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
         <v>326</v>
       </c>
@@ -4542,7 +4597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="8" t="s">
         <v>330</v>
       </c>
@@ -4568,7 +4623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>335</v>
       </c>
@@ -4586,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>337</v>
       </c>
@@ -4604,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -4622,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>340</v>
       </c>
@@ -4640,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>342</v>
       </c>
@@ -4656,7 +4711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>343</v>
       </c>
@@ -4676,6 +4731,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H138"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4692,16 +4748,16 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.28515625"/>
-    <col min="5" max="5" width="26.140625"/>
-    <col min="6" max="6" width="23.5703125"/>
-    <col min="7" max="7" width="70.28515625"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
+    <col min="4" max="4" width="20.26953125"/>
+    <col min="5" max="5" width="26.1796875"/>
+    <col min="6" max="6" width="23.54296875"/>
+    <col min="7" max="7" width="70.26953125"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4727,7 +4783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -4753,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -4779,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4801,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -4825,7 +4881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -4851,7 +4907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -4877,7 +4933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -4903,7 +4959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -4929,7 +4985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -4955,7 +5011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -4977,7 +5033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -5003,7 +5059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -5029,7 +5085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -5055,7 +5111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
@@ -5079,7 +5135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -5105,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -5131,7 +5187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -5157,7 +5213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -5181,7 +5237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -5203,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -5225,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -5251,7 +5307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -5273,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -5297,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -5323,7 +5379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -5349,7 +5405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -5375,7 +5431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -5397,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -5419,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -5441,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -5467,7 +5523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -5493,7 +5549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -5519,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -5541,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -5565,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -5591,7 +5647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -5617,7 +5673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -5643,7 +5699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -5669,7 +5725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -5695,7 +5751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -5721,7 +5777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -5747,7 +5803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -5773,7 +5829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -5799,7 +5855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -5825,7 +5881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -5851,7 +5907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -5877,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -5899,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -5921,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -5943,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -5965,7 +6021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -5987,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -6009,7 +6065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -6023,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -6049,7 +6105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>190</v>
       </c>
@@ -6069,7 +6125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -6095,7 +6151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>195</v>
       </c>
@@ -6121,7 +6177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>198</v>
       </c>
@@ -6147,7 +6203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>201</v>
       </c>
@@ -6173,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>205</v>
       </c>
@@ -6193,7 +6249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>207</v>
       </c>
@@ -6213,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -6233,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -6255,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>214</v>
       </c>
@@ -6281,7 +6337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -6303,7 +6359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
         <v>220</v>
       </c>
@@ -6329,7 +6385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>224</v>
       </c>
@@ -6355,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>228</v>
       </c>
@@ -6379,7 +6435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>230</v>
       </c>
@@ -6405,7 +6461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>234</v>
       </c>
@@ -6431,7 +6487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>238</v>
       </c>
@@ -6457,7 +6513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>241</v>
       </c>
@@ -6477,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>243</v>
       </c>
@@ -6503,7 +6559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>246</v>
       </c>
@@ -6529,7 +6585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>249</v>
       </c>
@@ -6555,7 +6611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>253</v>
       </c>
@@ -6581,7 +6637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>256</v>
       </c>
@@ -6607,7 +6663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>259</v>
       </c>
@@ -6633,7 +6689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="22" t="s">
         <v>262</v>
       </c>
@@ -6659,7 +6715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -6673,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -6687,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -6701,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -6715,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -6729,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -6743,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>266</v>
       </c>
@@ -6763,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -6777,7 +6833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -6803,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -6817,7 +6873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -6834,7 +6890,7 @@
       <c r="J91" s="21"/>
       <c r="K91" s="21"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -6851,7 +6907,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -6868,7 +6924,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -6882,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -6896,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -6910,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -6924,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -6938,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -6952,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -6966,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -6980,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -7004,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>275</v>
       </c>
@@ -7022,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7036,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7050,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -7064,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -7084,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -7098,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -7112,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -7126,7 +7182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>277</v>
       </c>
@@ -7148,7 +7204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -7162,7 +7218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -7176,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -7190,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -7204,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -7218,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -7232,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
         <v>279</v>
       </c>
@@ -7258,7 +7314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>284</v>
       </c>
@@ -7284,7 +7340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>288</v>
       </c>
@@ -7310,7 +7366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
         <v>292</v>
       </c>
@@ -7336,7 +7392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>296</v>
       </c>
@@ -7362,7 +7418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>300</v>
       </c>
@@ -7388,7 +7444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>304</v>
       </c>
@@ -7414,7 +7470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>308</v>
       </c>
@@ -7440,7 +7496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>312</v>
       </c>
@@ -7466,7 +7522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
         <v>316</v>
       </c>
@@ -7486,7 +7542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
         <v>320</v>
       </c>
@@ -7512,7 +7568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>324</v>
       </c>
@@ -7536,7 +7592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>326</v>
       </c>
@@ -7562,7 +7618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>330</v>
       </c>
@@ -7588,7 +7644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>343</v>
       </c>
@@ -7606,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>342</v>
       </c>
@@ -7622,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>340</v>
       </c>
@@ -7640,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -7658,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>337</v>
       </c>
@@ -7676,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>335</v>
       </c>
@@ -7696,6 +7752,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H137"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -7708,20 +7765,20 @@
   </sheetPr>
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="C94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.28515625"/>
-    <col min="5" max="5" width="26.140625"/>
-    <col min="6" max="6" width="23.5703125"/>
-    <col min="7" max="7" width="70.28515625"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
+    <col min="4" max="4" width="20.26953125"/>
+    <col min="5" max="5" width="26.1796875"/>
+    <col min="6" max="6" width="23.54296875"/>
+    <col min="7" max="7" width="70.26953125"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7747,7 +7804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -7773,7 +7830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -7799,7 +7856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -7812,7 +7869,9 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7821,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -7845,7 +7904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -7871,7 +7930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -7897,7 +7956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -7921,7 +7980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -7935,11 +7994,9 @@
         <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
         <v>39</v>
       </c>
@@ -7947,7 +8004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -7973,7 +8030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -7995,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -8021,7 +8078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -8047,7 +8104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -8073,31 +8130,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="27">
         <v>68</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="27">
         <v>13</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -8123,7 +8180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -8149,7 +8206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -8175,7 +8232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -8199,7 +8256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -8221,7 +8278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -8243,7 +8300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -8269,7 +8326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -8291,31 +8348,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="28">
         <v>1</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="28">
         <v>22</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="E24" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="29"/>
       <c r="H24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -8341,7 +8398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -8367,7 +8424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -8393,29 +8450,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="28">
         <v>14</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="28">
         <v>26</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="6"/>
+      <c r="E28" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -8437,7 +8494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -8459,7 +8516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -8485,7 +8542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -8511,7 +8568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -8537,7 +8594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -8559,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -8583,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -8609,7 +8666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -8635,7 +8692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -8661,7 +8718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -8687,7 +8744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -8713,7 +8770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -8739,7 +8796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -8765,7 +8822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -8791,7 +8848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -8817,7 +8874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -8843,7 +8900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -8869,7 +8926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -8895,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -8917,7 +8974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -8939,7 +8996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -8961,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -8983,7 +9040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -9005,7 +9062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -9027,7 +9084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -9041,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -9067,7 +9124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>190</v>
       </c>
@@ -9087,7 +9144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -9113,7 +9170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>195</v>
       </c>
@@ -9139,7 +9196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>198</v>
       </c>
@@ -9165,7 +9222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>201</v>
       </c>
@@ -9191,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>205</v>
       </c>
@@ -9211,7 +9268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>207</v>
       </c>
@@ -9231,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -9251,7 +9308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -9273,7 +9330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>214</v>
       </c>
@@ -9299,7 +9356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -9323,7 +9380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
         <v>220</v>
       </c>
@@ -9349,7 +9406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>224</v>
       </c>
@@ -9375,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>228</v>
       </c>
@@ -9399,7 +9456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>230</v>
       </c>
@@ -9425,7 +9482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>234</v>
       </c>
@@ -9451,7 +9508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>238</v>
       </c>
@@ -9477,7 +9534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>241</v>
       </c>
@@ -9497,7 +9554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>243</v>
       </c>
@@ -9523,7 +9580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>246</v>
       </c>
@@ -9549,7 +9606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>249</v>
       </c>
@@ -9575,7 +9632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>253</v>
       </c>
@@ -9601,7 +9658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>256</v>
       </c>
@@ -9627,7 +9684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>259</v>
       </c>
@@ -9653,7 +9710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="22" t="s">
         <v>262</v>
       </c>
@@ -9679,7 +9736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -9693,7 +9750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -9707,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -9721,7 +9778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -9735,7 +9792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -9749,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -9763,7 +9820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>266</v>
       </c>
@@ -9783,7 +9840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -9797,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -9823,7 +9880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -9837,7 +9894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -9854,7 +9911,7 @@
       <c r="J91" s="21"/>
       <c r="K91" s="21"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -9871,7 +9928,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -9888,7 +9945,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -9902,7 +9959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -9916,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -9930,7 +9987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -9944,7 +10001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -9958,7 +10015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -9972,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -9986,7 +10043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -10000,7 +10057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -10024,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>275</v>
       </c>
@@ -10035,14 +10092,16 @@
       <c r="D103" s="2">
         <v>101</v>
       </c>
-      <c r="E103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="F103" s="2"/>
       <c r="G103" s="6"/>
       <c r="H103" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -10056,7 +10115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -10070,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -10084,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -10104,7 +10163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -10118,7 +10177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -10132,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -10146,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>277</v>
       </c>
@@ -10158,17 +10217,15 @@
         <v>108</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -10182,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -10196,7 +10253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -10210,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -10224,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -10238,7 +10295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -10252,7 +10309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
         <v>279</v>
       </c>
@@ -10278,7 +10335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>284</v>
       </c>
@@ -10304,7 +10361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>288</v>
       </c>
@@ -10330,7 +10387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
         <v>292</v>
       </c>
@@ -10356,7 +10413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>296</v>
       </c>
@@ -10382,7 +10439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>300</v>
       </c>
@@ -10408,7 +10465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>304</v>
       </c>
@@ -10434,7 +10491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>308</v>
       </c>
@@ -10460,7 +10517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>312</v>
       </c>
@@ -10486,7 +10543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
         <v>316</v>
       </c>
@@ -10506,7 +10563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
         <v>320</v>
       </c>
@@ -10532,7 +10589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>324</v>
       </c>
@@ -10556,7 +10613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>326</v>
       </c>
@@ -10582,7 +10639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>330</v>
       </c>
@@ -10608,7 +10665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>343</v>
       </c>
@@ -10626,7 +10683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>342</v>
       </c>
@@ -10642,7 +10699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>340</v>
       </c>
@@ -10660,7 +10717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -10678,7 +10735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>337</v>
       </c>
@@ -10696,7 +10753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>335</v>
       </c>
@@ -10716,7 +10773,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H137"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge devt branch to move to 0.92.10 base
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc.VAIO\Documents\GitHub\Repetier-Firmware-0.92\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout for 1.0 and 2.0" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="354">
   <si>
     <t>NAME</t>
   </si>
@@ -1070,13 +1075,41 @@
   </si>
   <si>
     <t>PC24,135,6,Badge LED,  1 = On</t>
+  </si>
+  <si>
+    <t>Turn Table direction, 0=-, 1=+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>White Led Laser 1, 1=0n</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laser 2, 1 = 0N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn Table step</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn Table enable, 0 = enable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laser 1, 1 = ON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>White Led Laser 2, 1=ON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1096,8 +1129,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1194,6 +1233,18 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFC4BD97"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1222,7 +1273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1266,9 +1317,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1344,12 +1398,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1391,7 +1448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1426,7 +1483,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1644,20 +1701,18 @@
       <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125"/>
-    <col min="2" max="2" width="11.7109375"/>
-    <col min="3" max="3" width="8.7109375"/>
+    <col min="1" max="1" width="15.453125"/>
+    <col min="2" max="2" width="11.7265625"/>
     <col min="4" max="4" width="18"/>
-    <col min="5" max="5" width="46.5703125"/>
+    <col min="5" max="5" width="46.54296875"/>
     <col min="6" max="6" width="30"/>
-    <col min="7" max="7" width="71.7109375"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
-    <col min="9" max="1025" width="8.7109375"/>
+    <col min="7" max="7" width="71.7265625"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1757,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1781,7 +1836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1807,7 +1862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -1833,7 +1888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -1885,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -1911,7 +1966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1933,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -1959,7 +2014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -1985,7 +2040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -2011,7 +2066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
@@ -2035,7 +2090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -2061,7 +2116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -2087,7 +2142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -2113,7 +2168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -2139,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -2161,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -2183,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -2209,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -2231,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -2255,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -2281,7 +2336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -2307,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -2333,7 +2388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -2355,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -2377,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -2399,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -2425,7 +2480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -2451,7 +2506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -2477,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -2499,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -2523,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -2549,7 +2604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -2575,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -2601,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -2627,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -2653,7 +2708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -2679,7 +2734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -2705,7 +2760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -2757,7 +2812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -2783,7 +2838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -2809,7 +2864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -2835,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -2857,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -2879,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -2901,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -2923,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -2945,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -2967,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2981,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -3007,7 +3062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3021,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>190</v>
       </c>
@@ -3041,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>192</v>
       </c>
@@ -3067,7 +3122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>195</v>
       </c>
@@ -3093,7 +3148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>198</v>
       </c>
@@ -3119,7 +3174,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>201</v>
       </c>
@@ -3145,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -3165,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>207</v>
       </c>
@@ -3185,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>209</v>
       </c>
@@ -3205,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>211</v>
       </c>
@@ -3227,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>214</v>
       </c>
@@ -3253,7 +3308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>218</v>
       </c>
@@ -3275,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
         <v>220</v>
       </c>
@@ -3301,7 +3356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>224</v>
       </c>
@@ -3327,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>228</v>
       </c>
@@ -3351,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>230</v>
       </c>
@@ -3377,7 +3432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="15" t="s">
         <v>234</v>
       </c>
@@ -3403,7 +3458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>238</v>
       </c>
@@ -3429,7 +3484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>241</v>
       </c>
@@ -3449,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
         <v>243</v>
       </c>
@@ -3475,7 +3530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>246</v>
       </c>
@@ -3501,7 +3556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>249</v>
       </c>
@@ -3527,7 +3582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>253</v>
       </c>
@@ -3553,7 +3608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>256</v>
       </c>
@@ -3579,7 +3634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>259</v>
       </c>
@@ -3605,7 +3660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="22" t="s">
         <v>262</v>
       </c>
@@ -3631,7 +3686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3645,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3659,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3673,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3687,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3701,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3715,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="22" t="s">
         <v>266</v>
       </c>
@@ -3741,7 +3796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3755,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>269</v>
       </c>
@@ -3781,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3795,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3812,7 +3867,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3829,7 +3884,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3846,7 +3901,7 @@
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3860,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3874,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3888,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3902,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3916,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3930,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3944,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3958,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>272</v>
       </c>
@@ -3982,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>275</v>
       </c>
@@ -4000,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4014,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4028,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -4042,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>276</v>
       </c>
@@ -4062,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -4076,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -4090,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -4104,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>277</v>
       </c>
@@ -4126,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -4140,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -4154,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -4168,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -4182,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -4196,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -4210,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>279</v>
       </c>
@@ -4236,7 +4291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="23" t="s">
         <v>284</v>
       </c>
@@ -4262,7 +4317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="8" t="s">
         <v>288</v>
       </c>
@@ -4288,7 +4343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>292</v>
       </c>
@@ -4314,7 +4369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>296</v>
       </c>
@@ -4340,7 +4395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="24" t="s">
         <v>300</v>
       </c>
@@ -4366,7 +4421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>304</v>
       </c>
@@ -4392,7 +4447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>308</v>
       </c>
@@ -4418,7 +4473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="16" t="s">
         <v>312</v>
       </c>
@@ -4444,7 +4499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="24" t="s">
         <v>316</v>
       </c>
@@ -4470,7 +4525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
         <v>320</v>
       </c>
@@ -4496,7 +4551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>324</v>
       </c>
@@ -4516,7 +4571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
         <v>326</v>
       </c>
@@ -4542,7 +4597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="8" t="s">
         <v>330</v>
       </c>
@@ -4568,7 +4623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>335</v>
       </c>
@@ -4586,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>337</v>
       </c>
@@ -4604,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -4622,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>340</v>
       </c>
@@ -4640,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>342</v>
       </c>
@@ -4656,7 +4711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>343</v>
       </c>
@@ -4676,6 +4731,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H138"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4692,16 +4748,16 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.28515625"/>
-    <col min="5" max="5" width="26.140625"/>
-    <col min="6" max="6" width="23.5703125"/>
-    <col min="7" max="7" width="70.28515625"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
+    <col min="4" max="4" width="20.26953125"/>
+    <col min="5" max="5" width="26.1796875"/>
+    <col min="6" max="6" width="23.54296875"/>
+    <col min="7" max="7" width="70.26953125"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4727,7 +4783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -4753,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -4779,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4801,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -4825,7 +4881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -4851,7 +4907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -4877,7 +4933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -4903,7 +4959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -4929,7 +4985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -4955,7 +5011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -4977,7 +5033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -5003,7 +5059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -5029,7 +5085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -5055,7 +5111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
@@ -5079,7 +5135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -5105,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -5131,7 +5187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -5157,7 +5213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -5181,7 +5237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -5203,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -5225,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -5251,7 +5307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -5273,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -5297,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -5323,7 +5379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -5349,7 +5405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -5375,7 +5431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -5397,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -5419,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -5441,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -5467,7 +5523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -5493,7 +5549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -5519,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -5541,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -5565,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -5591,7 +5647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -5617,7 +5673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -5643,7 +5699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -5669,7 +5725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -5695,7 +5751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -5721,7 +5777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -5747,7 +5803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -5773,7 +5829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -5799,7 +5855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -5825,7 +5881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -5851,7 +5907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -5877,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -5899,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -5921,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -5943,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -5965,7 +6021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -5987,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -6009,7 +6065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -6023,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -6049,7 +6105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>190</v>
       </c>
@@ -6069,7 +6125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -6095,7 +6151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>195</v>
       </c>
@@ -6121,7 +6177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>198</v>
       </c>
@@ -6147,7 +6203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>201</v>
       </c>
@@ -6173,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>205</v>
       </c>
@@ -6193,7 +6249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>207</v>
       </c>
@@ -6213,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -6233,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -6255,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>214</v>
       </c>
@@ -6281,7 +6337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -6303,7 +6359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
         <v>220</v>
       </c>
@@ -6329,7 +6385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>224</v>
       </c>
@@ -6355,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>228</v>
       </c>
@@ -6379,7 +6435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>230</v>
       </c>
@@ -6405,7 +6461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>234</v>
       </c>
@@ -6431,7 +6487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>238</v>
       </c>
@@ -6457,7 +6513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>241</v>
       </c>
@@ -6477,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>243</v>
       </c>
@@ -6503,7 +6559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>246</v>
       </c>
@@ -6529,7 +6585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>249</v>
       </c>
@@ -6555,7 +6611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>253</v>
       </c>
@@ -6581,7 +6637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>256</v>
       </c>
@@ -6607,7 +6663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>259</v>
       </c>
@@ -6633,7 +6689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="22" t="s">
         <v>262</v>
       </c>
@@ -6659,7 +6715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -6673,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -6687,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -6701,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -6715,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -6729,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -6743,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>266</v>
       </c>
@@ -6763,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -6777,7 +6833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -6803,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -6817,7 +6873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -6834,7 +6890,7 @@
       <c r="J91" s="21"/>
       <c r="K91" s="21"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -6851,7 +6907,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -6868,7 +6924,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -6882,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -6896,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -6910,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -6924,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -6938,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -6952,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -6966,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -6980,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -7004,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>275</v>
       </c>
@@ -7022,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7036,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7050,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -7064,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -7084,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -7098,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -7112,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -7126,7 +7182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>277</v>
       </c>
@@ -7148,7 +7204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -7162,7 +7218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -7176,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -7190,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -7204,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -7218,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -7232,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
         <v>279</v>
       </c>
@@ -7258,7 +7314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>284</v>
       </c>
@@ -7284,7 +7340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>288</v>
       </c>
@@ -7310,7 +7366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
         <v>292</v>
       </c>
@@ -7336,7 +7392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>296</v>
       </c>
@@ -7362,7 +7418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>300</v>
       </c>
@@ -7388,7 +7444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>304</v>
       </c>
@@ -7414,7 +7470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>308</v>
       </c>
@@ -7440,7 +7496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>312</v>
       </c>
@@ -7466,7 +7522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
         <v>316</v>
       </c>
@@ -7486,7 +7542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
         <v>320</v>
       </c>
@@ -7512,7 +7568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>324</v>
       </c>
@@ -7536,7 +7592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>326</v>
       </c>
@@ -7562,7 +7618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>330</v>
       </c>
@@ -7588,7 +7644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>343</v>
       </c>
@@ -7606,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>342</v>
       </c>
@@ -7622,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>340</v>
       </c>
@@ -7640,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -7658,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>337</v>
       </c>
@@ -7676,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>335</v>
       </c>
@@ -7696,6 +7752,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H137"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -7708,20 +7765,20 @@
   </sheetPr>
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="C94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.28515625"/>
-    <col min="5" max="5" width="26.140625"/>
-    <col min="6" max="6" width="23.5703125"/>
-    <col min="7" max="7" width="70.28515625"/>
-    <col min="8" max="8" width="13.7109375" style="1"/>
+    <col min="4" max="4" width="20.26953125"/>
+    <col min="5" max="5" width="26.1796875"/>
+    <col min="6" max="6" width="23.54296875"/>
+    <col min="7" max="7" width="70.26953125"/>
+    <col min="8" max="8" width="13.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7747,7 +7804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -7773,7 +7830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -7799,7 +7856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -7812,7 +7869,9 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7821,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -7845,7 +7904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -7871,7 +7930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -7897,7 +7956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -7921,7 +7980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -7935,11 +7994,9 @@
         <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
         <v>39</v>
       </c>
@@ -7947,7 +8004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
@@ -7973,7 +8030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -7995,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
@@ -8021,7 +8078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>51</v>
       </c>
@@ -8047,7 +8104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -8073,31 +8130,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="27">
         <v>68</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="27">
         <v>13</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>63</v>
       </c>
@@ -8123,7 +8180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
@@ -8149,7 +8206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>71</v>
       </c>
@@ -8175,7 +8232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>75</v>
       </c>
@@ -8199,7 +8256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -8221,7 +8278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
@@ -8243,7 +8300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
@@ -8269,7 +8326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -8291,31 +8348,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="28">
         <v>1</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="28">
         <v>22</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="E24" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="29"/>
       <c r="H24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>89</v>
       </c>
@@ -8341,7 +8398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>91</v>
       </c>
@@ -8367,7 +8424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -8393,29 +8450,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="28">
         <v>14</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="28">
         <v>26</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="6"/>
+      <c r="E28" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
@@ -8437,7 +8494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -8459,7 +8516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>104</v>
       </c>
@@ -8485,7 +8542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>108</v>
       </c>
@@ -8511,7 +8568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -8537,7 +8594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>116</v>
       </c>
@@ -8559,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>118</v>
       </c>
@@ -8583,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>120</v>
       </c>
@@ -8609,7 +8666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>125</v>
       </c>
@@ -8635,7 +8692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -8661,7 +8718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
@@ -8687,7 +8744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>140</v>
       </c>
@@ -8713,7 +8770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>145</v>
       </c>
@@ -8739,7 +8796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
@@ -8765,7 +8822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>155</v>
       </c>
@@ -8791,7 +8848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>160</v>
       </c>
@@ -8817,7 +8874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>164</v>
       </c>
@@ -8843,7 +8900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -8869,7 +8926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
@@ -8895,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>174</v>
       </c>
@@ -8917,7 +8974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>176</v>
       </c>
@@ -8939,7 +8996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>178</v>
       </c>
@@ -8961,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -8983,7 +9040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -9005,7 +9062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -9027,7 +9084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -9041,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>186</v>
       </c>
@@ -9067,7 +9124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>190</v>
       </c>
@@ -9087,7 +9144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -9113,7 +9170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>195</v>
       </c>
@@ -9139,7 +9196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>198</v>
       </c>
@@ -9165,7 +9222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>201</v>
       </c>
@@ -9191,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>205</v>
       </c>
@@ -9211,7 +9268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>207</v>
       </c>
@@ -9231,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -9251,7 +9308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -9273,7 +9330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>214</v>
       </c>
@@ -9299,7 +9356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -9323,7 +9380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
         <v>220</v>
       </c>
@@ -9349,7 +9406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>224</v>
       </c>
@@ -9375,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>228</v>
       </c>
@@ -9399,7 +9456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>230</v>
       </c>
@@ -9425,7 +9482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>234</v>
       </c>
@@ -9451,7 +9508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>238</v>
       </c>
@@ -9477,7 +9534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>241</v>
       </c>
@@ -9497,7 +9554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>243</v>
       </c>
@@ -9523,7 +9580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>246</v>
       </c>
@@ -9549,7 +9606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>249</v>
       </c>
@@ -9575,7 +9632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>253</v>
       </c>
@@ -9601,7 +9658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>256</v>
       </c>
@@ -9627,7 +9684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>259</v>
       </c>
@@ -9653,7 +9710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="22" t="s">
         <v>262</v>
       </c>
@@ -9679,7 +9736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -9693,7 +9750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -9707,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -9721,7 +9778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -9735,7 +9792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -9749,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -9763,7 +9820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>266</v>
       </c>
@@ -9783,7 +9840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -9797,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -9823,7 +9880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -9837,7 +9894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -9854,7 +9911,7 @@
       <c r="J91" s="21"/>
       <c r="K91" s="21"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -9871,7 +9928,7 @@
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -9888,7 +9945,7 @@
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -9902,7 +9959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -9916,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -9930,7 +9987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -9944,7 +10001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -9958,7 +10015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -9972,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -9986,7 +10043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -10000,7 +10057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -10024,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>275</v>
       </c>
@@ -10035,14 +10092,16 @@
       <c r="D103" s="2">
         <v>101</v>
       </c>
-      <c r="E103" s="2"/>
+      <c r="E103" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="F103" s="2"/>
       <c r="G103" s="6"/>
       <c r="H103" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -10056,7 +10115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -10070,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -10084,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>276</v>
       </c>
@@ -10104,7 +10163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -10118,7 +10177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -10132,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -10146,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>277</v>
       </c>
@@ -10158,17 +10217,15 @@
         <v>108</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -10182,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -10196,7 +10253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -10210,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -10224,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -10238,7 +10295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -10252,7 +10309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
         <v>279</v>
       </c>
@@ -10278,7 +10335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>284</v>
       </c>
@@ -10304,7 +10361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>288</v>
       </c>
@@ -10330,7 +10387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
         <v>292</v>
       </c>
@@ -10356,7 +10413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
         <v>296</v>
       </c>
@@ -10382,7 +10439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
         <v>300</v>
       </c>
@@ -10408,7 +10465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>304</v>
       </c>
@@ -10434,7 +10491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>308</v>
       </c>
@@ -10460,7 +10517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>312</v>
       </c>
@@ -10486,7 +10543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
         <v>316</v>
       </c>
@@ -10506,7 +10563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
         <v>320</v>
       </c>
@@ -10532,7 +10589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>324</v>
       </c>
@@ -10556,7 +10613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>326</v>
       </c>
@@ -10582,7 +10639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>330</v>
       </c>
@@ -10608,7 +10665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>343</v>
       </c>
@@ -10626,7 +10683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>342</v>
       </c>
@@ -10642,7 +10699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>340</v>
       </c>
@@ -10660,7 +10717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>339</v>
       </c>
@@ -10678,7 +10735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>337</v>
       </c>
@@ -10696,7 +10753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>335</v>
       </c>
@@ -10716,7 +10773,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H137"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>